<commit_message>
excel writer date impl
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -1,24 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semihunaldi/DEV/ExcelOrm/src/main/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>name</t>
   </si>
@@ -165,13 +157,46 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>13/08/2017 14:37</t>
+  </si>
+  <si>
+    <t>13/08/2017 14:42</t>
+  </si>
+  <si>
+    <t>13/08/2017 14:43</t>
+  </si>
+  <si>
+    <t>13/08/2017 14:44</t>
+  </si>
+  <si>
+    <t>13/08/2017 14:46</t>
+  </si>
+  <si>
+    <t>14/08/2017 14:38</t>
+  </si>
+  <si>
+    <t>15/08/2017 14:39</t>
+  </si>
+  <si>
+    <t>16/08/2017 14:40</t>
+  </si>
+  <si>
+    <t>17/08/2017 14:41</t>
+  </si>
+  <si>
+    <t>22/08/2017 14:45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d/m/yyyy\ h:mm"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,16 +515,16 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.296875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +544,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -535,11 +560,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="3">
-        <v>42959.592361111114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -555,11 +580,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="3">
-        <v>42960.592361111114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -575,11 +600,11 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3">
-        <v>42961.592361111114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -595,11 +620,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3">
-        <v>42962.592361111114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -615,12 +640,12 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3">
-        <v>42963.592361111114</v>
+      <c r="F6" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -636,11 +661,11 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3">
-        <v>42964.592361111114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -656,11 +681,11 @@
       <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="3">
-        <v>42965.592361111114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -676,11 +701,11 @@
       <c r="E9" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="3">
-        <v>42966.592361111114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -696,11 +721,11 @@
       <c r="E10" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="3">
-        <v>42967.592361111114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -716,11 +741,12 @@
       <c r="E11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="3">
-        <v>42968.592361111114</v>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
migrated to sheetName from sheet index while reading/writing excel
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semihunaldi/DEV/ExcelOrm/src/main/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="636" yWindow="1176" windowWidth="28164" windowHeight="13176" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="13180" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -194,9 +202,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m/yyyy\ h:mm"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,13 +526,13 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="16.296875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +552,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -564,7 +572,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -584,7 +592,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -604,7 +612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -624,7 +632,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -645,7 +653,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -665,7 +673,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -685,7 +693,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -705,7 +713,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -725,7 +733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
reading excel with multiple sheets test added
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="13180" tabRatio="500"/>
+    <workbookView xWindow="5980" yWindow="8120" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="People" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -195,6 +196,36 @@
   </si>
   <si>
     <t>22/08/2017 14:45</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>name1</t>
+  </si>
+  <si>
+    <t>surname1</t>
+  </si>
+  <si>
+    <t>name2</t>
+  </si>
+  <si>
+    <t>surname2</t>
+  </si>
+  <si>
+    <t>name3</t>
+  </si>
+  <si>
+    <t>surname3</t>
+  </si>
+  <si>
+    <t>name4</t>
+  </si>
+  <si>
+    <t>surname4</t>
   </si>
 </sst>
 </file>
@@ -522,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -757,4 +788,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel reading/writing adjustments for multiple sheets and abnormal data placement in excel.
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="8120" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5440" yWindow="6920" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="People" sheetId="2" r:id="rId2"/>
+    <sheet name="TaskMiddle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -554,7 +555,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -843,4 +844,242 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E3:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel cells as formatted Numeric date, causes problems when parsing. Now it is looking the cell type before parsing date.
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="6920" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3500" yWindow="3360" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="People" sheetId="2" r:id="rId2"/>
-    <sheet name="TaskMiddle" sheetId="3" r:id="rId3"/>
+    <sheet name="DateTask" sheetId="4" r:id="rId2"/>
+    <sheet name="People" sheetId="2" r:id="rId3"/>
+    <sheet name="TaskMiddle" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -270,11 +271,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +558,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+      <selection activeCell="F11" sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,6 +795,244 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5">
+        <v>42783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5">
+        <v>42784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5">
+        <v>42785</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5">
+        <v>42786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5">
+        <v>42787</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="5">
+        <v>42788</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="5">
+        <v>42789</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="5">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="5">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="5">
+        <v>42792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -846,11 +1087,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excel read/write enum implementation
</commit_message>
<xml_diff>
--- a/src/main/resources/TaskExcel.xlsx
+++ b/src/main/resources/TaskExcel.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="3360" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3400" yWindow="7400" windowWidth="28160" windowHeight="13180" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="DateTask" sheetId="4" r:id="rId2"/>
-    <sheet name="People" sheetId="2" r:id="rId3"/>
-    <sheet name="TaskMiddle" sheetId="3" r:id="rId4"/>
+    <sheet name="EnumTaskTest" sheetId="5" r:id="rId2"/>
+    <sheet name="DateTask" sheetId="4" r:id="rId3"/>
+    <sheet name="People" sheetId="2" r:id="rId4"/>
+    <sheet name="TaskMiddle" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -228,6 +229,15 @@
   </si>
   <si>
     <t>surname4</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>FINISHED</t>
   </si>
 </sst>
 </file>
@@ -796,10 +806,281 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1087,7 +1368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:J13"/>
   <sheetViews>

</xml_diff>